<commit_message>
Updated all on 20Feb
</commit_message>
<xml_diff>
--- a/pages/STPTestData.xlsx
+++ b/pages/STPTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Serole Automation\playwright_python\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F172B42-F91C-4B98-A3EC-1B26C99070A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05239AB3-EDC1-4F48-93A3-949456D4AA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{45C1E7C0-1AF2-45CB-BEA8-DD612E61CE1D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>RegNo</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>751211-14-5267</t>
+  </si>
+  <si>
+    <t>BFJ7088</t>
+  </si>
+  <si>
+    <t>940314-11-5725</t>
+  </si>
+  <si>
+    <t>PC NSTP</t>
   </si>
 </sst>
 </file>
@@ -180,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -188,7 +197,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,11 +511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689C8A9F-98AE-49F8-89B3-BABBB35DE82F}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:B11"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,14 +633,26 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>